<commit_message>
Added better support for custom fields
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments_multi_currency.xlsx
+++ b/public/sample_uploads/capital_commitments_multi_currency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3536A35A-5936-4EC0-8C3B-49C07061564C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7645FDDE-B012-467D-870A-C8B97553B5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R9"/>
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed issue with setup of FCF in imports
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments_multi_currency.xlsx
+++ b/public/sample_uploads/capital_commitments_multi_currency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2442A02-5AAC-41DA-BCA9-486CF26AA0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC0FA6E-6297-4979-95A0-D0E3E621BC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>KYC Investing Entity</t>
+  </si>
+  <si>
+    <t>CF1</t>
+  </si>
+  <si>
+    <t>CF2</t>
+  </si>
+  <si>
+    <t>CF3</t>
   </si>
 </sst>
 </file>
@@ -519,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -539,7 +548,7 @@
     <col min="16" max="16" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -594,8 +603,17 @@
       <c r="R1" t="s">
         <v>35</v>
       </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -644,8 +662,11 @@
       <c r="R2" t="s">
         <v>36</v>
       </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,8 +703,11 @@
       <c r="R3" t="s">
         <v>36</v>
       </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -720,8 +744,11 @@
       <c r="R4" t="s">
         <v>36</v>
       </c>
+      <c r="S4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -770,8 +797,11 @@
       <c r="R5" t="s">
         <v>36</v>
       </c>
+      <c r="S5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -808,8 +838,11 @@
       <c r="R6" t="s">
         <v>36</v>
       </c>
+      <c r="S6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -846,8 +879,11 @@
       <c r="R7" t="s">
         <v>36</v>
       </c>
+      <c r="S7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -884,8 +920,11 @@
       <c r="R8" t="s">
         <v>36</v>
       </c>
+      <c r="S8">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -921,6 +960,9 @@
       </c>
       <c r="R9" t="s">
         <v>36</v>
+      </c>
+      <c r="S9">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fied import investor access
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_commitments_multi_currency.xlsx
+++ b/public/sample_uploads/capital_commitments_multi_currency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DC0FA6E-6297-4979-95A0-D0E3E621BC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AA6BC7-65CA-4C46-BA41-3E8D88799FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>SAAS Fund</t>
   </si>
@@ -147,13 +147,37 @@
     <t>KYC Investing Entity</t>
   </si>
   <si>
-    <t>CF1</t>
-  </si>
-  <si>
-    <t>CF2</t>
-  </si>
-  <si>
-    <t>CF3</t>
+    <t>CF 1</t>
+  </si>
+  <si>
+    <t>CF 2</t>
+  </si>
+  <si>
+    <t>CF 3</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -531,7 +555,7 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="U2" sqref="U2:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -665,6 +689,12 @@
       <c r="S2">
         <v>1</v>
       </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -706,6 +736,12 @@
       <c r="S3">
         <v>2</v>
       </c>
+      <c r="T3" t="s">
+        <v>42</v>
+      </c>
+      <c r="U3">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -747,6 +783,12 @@
       <c r="S4">
         <v>3</v>
       </c>
+      <c r="T4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U4">
+        <v>300</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -800,6 +842,12 @@
       <c r="S5">
         <v>4</v>
       </c>
+      <c r="T5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5">
+        <v>400</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -841,6 +889,12 @@
       <c r="S6">
         <v>5</v>
       </c>
+      <c r="T6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6">
+        <v>500</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -882,6 +936,12 @@
       <c r="S7">
         <v>6</v>
       </c>
+      <c r="T7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U7">
+        <v>600</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -923,6 +983,12 @@
       <c r="S8">
         <v>7</v>
       </c>
+      <c r="T8" t="s">
+        <v>47</v>
+      </c>
+      <c r="U8">
+        <v>700</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -963,6 +1029,12 @@
       </c>
       <c r="S9">
         <v>8</v>
+      </c>
+      <c r="T9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9">
+        <v>800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>